<commit_message>
feat(source): improve the output variables file
</commit_message>
<xml_diff>
--- a/AquatoxBasedOptimization/OutputVariables.xlsx
+++ b/AquatoxBasedOptimization/OutputVariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanry\Documents\Repositories\AquatoxBasedOptimization\AquatoxBasedOptimization\AquatoxBasedOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanry\Documents\AquatoxBasedOptimization\AquatoxBasedOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B28FDB13-37E8-4E3E-8674-CE0F8B2DB7B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1E75F5-2CEA-48D7-A101-89805976E257}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13332" windowHeight="5400" xr2:uid="{3A4D8659-4295-454E-BF5F-02CAD0D5AEEA}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3A4D8659-4295-454E-BF5F-02CAD0D5AEEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Oxygen</t>
   </si>
@@ -42,16 +42,32 @@
   </si>
   <si>
     <t>Secchi d</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>Phyto. Chlorophyll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,13 +410,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5EAFE89-4CAB-4786-9642-6E400CE21525}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.5234375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -425,7 +445,32 @@
         <v>560</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>552</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>